<commit_message>
Continued implementing script. Added database file
</commit_message>
<xml_diff>
--- a/Database/Stonks Animal Crossing.xlsx
+++ b/Database/Stonks Animal Crossing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miguel\Documents\Python Projects\Animal Crossing Turnips\turnipCalculator\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F778D62B-491C-4F67-AC9B-A0A8578498BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DFDA769-B291-4F29-AF90-6AFCC44FE96D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4FE20F5E-B891-4B21-9DC0-A68B8C5A81BF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4FE20F5E-B891-4B21-9DC0-A68B8C5A81BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>Semana 1</t>
   </si>
@@ -185,6 +185,9 @@
   </si>
   <si>
     <t>Miércoles M</t>
+  </si>
+  <si>
+    <t>Big Spike'</t>
   </si>
 </sst>
 </file>
@@ -436,7 +439,7 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -472,6 +475,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="15" borderId="3" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -706,8 +712,29 @@
                 <c:pt idx="3">
                   <c:v>452</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>121.30000000000001</c:v>
+                </c:pt>
                 <c:pt idx="5">
                   <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>78</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4853,8 +4880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2A28895-8293-452B-BB3B-D8280B6AFD24}">
   <dimension ref="B2:P33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4865,30 +4892,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="15" t="s">
+      <c r="D2" s="15"/>
+      <c r="E2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="16" t="s">
+      <c r="F2" s="16"/>
+      <c r="G2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="16"/>
-      <c r="I2" s="17" t="s">
+      <c r="H2" s="17"/>
+      <c r="I2" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="17"/>
-      <c r="K2" s="18" t="s">
+      <c r="J2" s="18"/>
+      <c r="K2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="18"/>
-      <c r="M2" s="13" t="s">
+      <c r="L2" s="19"/>
+      <c r="M2" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="13"/>
+      <c r="N2" s="14"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C3" s="5" t="s">
@@ -4950,20 +4977,37 @@
       <c r="F4" s="4">
         <v>452</v>
       </c>
-      <c r="G4" s="3"/>
+      <c r="G4" s="3">
+        <f>(F4*0.4+H4*0.6)/2</f>
+        <v>121.30000000000001</v>
+      </c>
       <c r="H4" s="4">
         <v>103</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="4"/>
+      <c r="I4" s="3">
+        <v>76</v>
+      </c>
+      <c r="J4" s="4">
+        <v>80</v>
+      </c>
+      <c r="K4" s="3">
+        <v>78</v>
+      </c>
+      <c r="L4" s="4">
+        <v>54</v>
+      </c>
+      <c r="M4" s="3">
+        <v>65</v>
+      </c>
+      <c r="N4" s="4">
+        <v>78</v>
+      </c>
       <c r="O4" s="2">
         <v>105</v>
       </c>
-      <c r="P4" s="2"/>
+      <c r="P4" s="13" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
@@ -5534,7 +5578,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BADF433-E7F4-4D8F-A740-A6D1089EC5B1}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added new database to the repository
Signed-off-by: Miguel Crespo <crespomiguel93@gmail.com>
</commit_message>
<xml_diff>
--- a/Database/Stonks Animal Crossing.xlsx
+++ b/Database/Stonks Animal Crossing.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miguel\Documents\Python Projects\Animal Crossing Turnips\turnipCalculator\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DFDA769-B291-4F29-AF90-6AFCC44FE96D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AFD50A4-EA23-46A3-A3D2-3E367E885A7E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4FE20F5E-B891-4B21-9DC0-A68B8C5A81BF}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="52">
   <si>
     <t>Semana 1</t>
   </si>
@@ -188,6 +188,9 @@
   </si>
   <si>
     <t>Big Spike'</t>
+  </si>
+  <si>
+    <t>Decreasing'</t>
   </si>
 </sst>
 </file>
@@ -713,7 +716,7 @@
                   <c:v>452</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>121.30000000000001</c:v>
+                  <c:v>190</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>103</c:v>
@@ -834,6 +837,42 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>48</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -932,6 +971,42 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>319</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>59</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1030,6 +1105,42 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>47</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1128,6 +1239,27 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>496</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>206</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>104</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4881,12 +5013,14 @@
   <dimension ref="B2:P33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="14" width="11.42578125" style="1"/>
+    <col min="1" max="6" width="11.42578125" style="1"/>
+    <col min="7" max="7" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="14" width="11.42578125" style="1"/>
     <col min="15" max="15" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16384" width="11.42578125" style="1"/>
   </cols>
@@ -4978,8 +5112,8 @@
         <v>452</v>
       </c>
       <c r="G4" s="3">
-        <f>(F4*0.4+H4*0.6)/2</f>
-        <v>121.30000000000001</v>
+        <f>ROUND(F4*0.25+H4*0.75,0)</f>
+        <v>190</v>
       </c>
       <c r="H4" s="4">
         <v>103</v>
@@ -5013,77 +5147,181 @@
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
+      <c r="C5" s="3">
+        <v>97</v>
+      </c>
+      <c r="D5" s="4">
+        <v>92</v>
+      </c>
+      <c r="E5" s="3">
+        <v>87</v>
+      </c>
+      <c r="F5" s="4">
+        <v>83</v>
+      </c>
+      <c r="G5" s="3">
+        <v>78</v>
+      </c>
+      <c r="H5" s="4">
+        <v>75</v>
+      </c>
+      <c r="I5" s="3">
+        <v>69</v>
+      </c>
+      <c r="J5" s="4">
+        <v>63</v>
+      </c>
+      <c r="K5" s="3">
+        <v>60</v>
+      </c>
+      <c r="L5" s="4">
+        <v>55</v>
+      </c>
+      <c r="M5" s="3">
+        <v>52</v>
+      </c>
+      <c r="N5" s="4">
+        <v>48</v>
+      </c>
+      <c r="O5" s="2">
+        <v>108</v>
+      </c>
+      <c r="P5" s="13" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
+      <c r="C6" s="3">
+        <v>93</v>
+      </c>
+      <c r="D6" s="4">
+        <v>88</v>
+      </c>
+      <c r="E6" s="3">
+        <v>83</v>
+      </c>
+      <c r="F6" s="4">
+        <v>79</v>
+      </c>
+      <c r="G6" s="3">
+        <v>75</v>
+      </c>
+      <c r="H6" s="4">
+        <v>71</v>
+      </c>
+      <c r="I6" s="3">
+        <v>121</v>
+      </c>
+      <c r="J6" s="4">
+        <v>160</v>
+      </c>
+      <c r="K6" s="3">
+        <v>319</v>
+      </c>
+      <c r="L6" s="4">
+        <f>ROUND(0.4*K6+0.6*M6,0)</f>
+        <v>195</v>
+      </c>
+      <c r="M6" s="3">
+        <v>113</v>
+      </c>
+      <c r="N6" s="4">
+        <v>59</v>
+      </c>
+      <c r="O6" s="2">
+        <v>104</v>
+      </c>
+      <c r="P6" s="13" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
+      <c r="C7" s="3">
+        <v>94</v>
+      </c>
+      <c r="D7" s="4">
+        <v>90</v>
+      </c>
+      <c r="E7" s="3">
+        <v>86</v>
+      </c>
+      <c r="F7" s="4">
+        <v>82</v>
+      </c>
+      <c r="G7" s="3">
+        <v>78</v>
+      </c>
+      <c r="H7" s="4">
+        <v>75</v>
+      </c>
+      <c r="I7" s="3">
+        <v>63</v>
+      </c>
+      <c r="J7" s="4">
+        <v>60</v>
+      </c>
+      <c r="K7" s="4">
+        <f>ROUND(0.4*J7+0.6*L7,0)</f>
+        <v>58</v>
+      </c>
+      <c r="L7" s="4">
+        <v>56</v>
+      </c>
+      <c r="M7" s="3">
+        <v>50</v>
+      </c>
+      <c r="N7" s="4">
+        <v>47</v>
+      </c>
+      <c r="O7" s="2">
+        <v>106</v>
+      </c>
+      <c r="P7" s="13" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="3"/>
+      <c r="C8" s="3">
+        <v>91</v>
+      </c>
+      <c r="D8" s="4">
+        <v>88</v>
+      </c>
+      <c r="E8" s="3">
+        <v>113</v>
+      </c>
+      <c r="F8" s="4">
+        <v>160</v>
+      </c>
+      <c r="G8" s="3">
+        <v>496</v>
+      </c>
+      <c r="H8" s="4">
+        <v>206</v>
+      </c>
+      <c r="I8" s="3">
+        <v>104</v>
+      </c>
       <c r="J8" s="4"/>
       <c r="K8" s="3"/>
       <c r="L8" s="4"/>
       <c r="M8" s="3"/>
       <c r="N8" s="4"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
+      <c r="O8" s="2">
+        <v>103</v>
+      </c>
+      <c r="P8" s="13" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">

</xml_diff>

<commit_message>
Included Deep Learning Turnip Calculator
</commit_message>
<xml_diff>
--- a/Database/Stonks Animal Crossing.xlsx
+++ b/Database/Stonks Animal Crossing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miguel\Documents\Python Projects\Animal Crossing Turnips\turnipCalculator\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92189731-F6F0-4BE0-BBB3-514B9C425DCC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA57F0F6-4EDA-41D8-A53A-FEC54CACA17D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4FE20F5E-B891-4B21-9DC0-A68B8C5A81BF}"/>
   </bookViews>
@@ -1266,6 +1266,9 @@
                 <c:pt idx="8">
                   <c:v>79</c:v>
                 </c:pt>
+                <c:pt idx="10">
+                  <c:v>73</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1364,6 +1367,12 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>117</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5019,7 +5028,7 @@
   <dimension ref="B2:P33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5324,7 +5333,9 @@
         <v>79</v>
       </c>
       <c r="L8" s="4"/>
-      <c r="M8" s="3"/>
+      <c r="M8" s="3">
+        <v>73</v>
+      </c>
       <c r="N8" s="4"/>
       <c r="O8" s="2">
         <v>103</v>
@@ -5337,8 +5348,12 @@
       <c r="B9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="4"/>
+      <c r="C9" s="3">
+        <v>89</v>
+      </c>
+      <c r="D9" s="4">
+        <v>117</v>
+      </c>
       <c r="E9" s="3"/>
       <c r="F9" s="4"/>
       <c r="G9" s="3"/>
@@ -5349,7 +5364,9 @@
       <c r="L9" s="4"/>
       <c r="M9" s="3"/>
       <c r="N9" s="4"/>
-      <c r="O9" s="2"/>
+      <c r="O9" s="2">
+        <v>94</v>
+      </c>
       <c r="P9" s="2"/>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">

</xml_diff>